<commit_message>
mise à jour du rapport de projet
le rapport de projet à été mis à jour.
</commit_message>
<xml_diff>
--- a/Documentations/Fishermen - Planification initiale - KGN.xlsx
+++ b/Documentations/Fishermen - Planification initiale - KGN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningProjet" sheetId="11" r:id="rId1"/>
@@ -2997,9 +2997,9 @@
   </sheetPr>
   <dimension ref="A1:AP28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="C3" s="41">
         <f ca="1">TODAY()</f>
-        <v>44705</v>
+        <v>44711</v>
       </c>
       <c r="D3" s="42"/>
       <c r="E3" s="35"/>
@@ -3057,7 +3057,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="43">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="36"/>
@@ -4307,7 +4307,9 @@
       <c r="E25" s="39">
         <v>44705</v>
       </c>
-      <c r="F25" s="23"/>
+      <c r="F25" s="23">
+        <v>44705</v>
+      </c>
       <c r="G25" s="13">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -5101,26 +5103,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5408,6 +5390,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
@@ -5417,25 +5419,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5454,4 +5437,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>